<commit_message>
areas de registro en angular
</commit_message>
<xml_diff>
--- a/src/assets/formatos/Formato Carga de Alumnos.xlsx
+++ b/src/assets/formatos/Formato Carga de Alumnos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TESI Indicadores\Website Angular\Tesi-Indicadores-FrontEnd\src\assets\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFCFCE2-391A-4B82-9923-5F27A370F17C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE28E0E7-62D6-4B2B-95CB-728CB0029415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E186D6C7-C6D6-47B6-9AF2-264C7F877308}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Formato" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Formato!$A$1:$F$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Formato!$A$1:$F$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>No.</t>
   </si>
@@ -42,13 +42,22 @@
     <t>Carrera</t>
   </si>
   <si>
-    <t>Formato para la Carga de Usuarios.                                                           (Nota no Modificar los nombres de las columnas)</t>
-  </si>
-  <si>
     <t>Matricula</t>
   </si>
   <si>
     <t>Grupo</t>
+  </si>
+  <si>
+    <t>Formato para la Carga de Alumnos.                                                           (Nota no Modificar los nombres de las columnas)</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>ISC</t>
   </si>
 </sst>
 </file>
@@ -105,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -136,21 +145,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -159,20 +153,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -202,13 +188,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -245,13 +231,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -288,13 +274,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -331,13 +317,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -374,13 +360,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -417,13 +403,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -460,13 +446,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -503,13 +489,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -546,13 +532,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -589,13 +575,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -632,13 +618,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -675,13 +661,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -718,13 +704,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>132720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1107,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9229E7-13F4-4225-BBED-27D055220375}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1125,266 +1111,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="30.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" ht="30.75" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>201224992</v>
+      </c>
+      <c r="E3">
+        <v>1802</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Agregando links de descargas de formatos
</commit_message>
<xml_diff>
--- a/src/assets/formatos/Formato Carga de Alumnos.xlsx
+++ b/src/assets/formatos/Formato Carga de Alumnos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TESI Indicadores\Website Angular\Tesi-Indicadores-FrontEnd\src\assets\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE28E0E7-62D6-4B2B-95CB-728CB0029415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5CC6FC-3076-4A44-85D1-D906CE8EFDEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E186D6C7-C6D6-47B6-9AF2-264C7F877308}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>No.</t>
   </si>
@@ -49,15 +49,6 @@
   </si>
   <si>
     <t>Formato para la Carga de Alumnos.                                                           (Nota no Modificar los nombres de las columnas)</t>
-  </si>
-  <si>
-    <t>Mario</t>
-  </si>
-  <si>
-    <t>Alberto</t>
-  </si>
-  <si>
-    <t>ISC</t>
   </si>
 </sst>
 </file>
@@ -1093,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9229E7-13F4-4225-BBED-27D055220375}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1140,26 +1131,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>201224992</v>
-      </c>
-      <c r="E3">
-        <v>1802</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
@@ -1171,6 +1142,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005E2DB502ABF570459D92EAB368475EB9" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc33ec95a03d3916ee7c550885e77c05">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aa9ecf5a-f88a-4c81-95fd-fe1157aac7ad" xmlns:ns4="112e49ae-75ca-444f-98be-3b3ec7e22459" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9408b6cd564dfbdec8defa50352aa754" ns3:_="" ns4:_="">
     <xsd:import namespace="aa9ecf5a-f88a-4c81-95fd-fe1157aac7ad"/>
@@ -1341,15 +1321,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1357,6 +1328,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60FEB2BC-FDC5-4E40-9D1B-465E85B3F859}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D91726C-1B1F-487D-8645-98B7DB2DCA99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1371,14 +1350,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60FEB2BC-FDC5-4E40-9D1B-465E85B3F859}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>